<commit_message>
fixed error - cant concatenate str to list(print2Both was culprit) and added some assets
</commit_message>
<xml_diff>
--- a/allScouts.xlsx
+++ b/allScouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asr31\Documents\GitHub\pesmobile_bluestacks_pyautogui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76497DBC-2D6F-47D9-B679-5B5950B1FDAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628CE19F-1191-4070-9591-C73C85E72147}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="0" windowWidth="28260" windowHeight="12810" xr2:uid="{E9352122-6993-43C4-A58C-32BB48012C89}"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="28260" windowHeight="12810" xr2:uid="{E9352122-6993-43C4-A58C-32BB48012C89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Other (Europe)</t>
   </si>
@@ -249,9 +249,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>Po</t>
-  </si>
-  <si>
     <t>trol</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>Util</t>
-  </si>
-  <si>
     <t>USE COLOURS AT ALL TIMES</t>
   </si>
   <si>
@@ -302,12 +296,15 @@
   <si>
     <t>league\n(Asia)</t>
   </si>
+  <si>
+    <t>Ki</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +352,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -377,19 +402,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2334F5-37B0-42FC-B6A3-5B3D3A1EDA71}">
-  <dimension ref="A1:G4356"/>
+  <dimension ref="A1:I4356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,11 +749,11 @@
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>87</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>85</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -735,9 +763,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -747,14 +775,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
-      <c r="B3">
-        <v>18</v>
+      <c r="B3" t="s">
+        <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -764,14 +792,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
-      <c r="B4">
-        <v>25</v>
+      <c r="B4" t="s">
+        <v>74</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -781,224 +809,245 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
-      <c r="B5">
-        <v>30</v>
+      <c r="B5" t="s">
+        <v>63</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>88</v>
+      <c r="G6" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>91</v>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>90</v>
+      <c r="F12" s="4" t="s">
+        <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>89</v>
+      <c r="F13" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>78</v>
@@ -1008,101 +1057,77 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>86</v>
-      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
     </row>

</xml_diff>